<commit_message>
Fixed a bad reference in data export in aL extract. Added line in ellipsoid to fix bad segmentation error in reflexed plane systems.
</commit_message>
<xml_diff>
--- a/scripts_python/references/ref_MD_backup.xlsx
+++ b/scripts_python/references/ref_MD_backup.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="8">
   <si>
     <t xml:space="preserve">Referencias</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t xml:space="preserve">CsCl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MgZn2</t>
   </si>
 </sst>
 </file>
@@ -121,7 +124,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -248,114 +251,270 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="A7:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.25"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>0.423</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>-94</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <v>-50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>0.47</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>16</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>-48</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>-36</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>0.511</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>-29</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>-16</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>0.73</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>-16</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>0.76</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
         <v>-14</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>-4</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>0.852</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>-10</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>0.815</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>-8</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>0.782</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>0.69</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>-4</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>0.758</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>-19</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>0.692</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>-24</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>0.797</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>-19</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>0.673</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>-16</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added AlB2 and CaCu5 ref F for MD.
</commit_message>
<xml_diff>
--- a/scripts_python/references/ref_MD_backup.xlsx
+++ b/scripts_python/references/ref_MD_backup.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="10">
   <si>
     <t xml:space="preserve">Referencias</t>
   </si>
@@ -44,6 +44,12 @@
   </si>
   <si>
     <t xml:space="preserve">MgZn2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AlB2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CaCu5</t>
   </si>
 </sst>
 </file>
@@ -56,7 +62,7 @@
   <fonts count="4">
     <font>
       <sz val="10"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
@@ -119,7 +125,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -128,138 +134,38 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
-  <a:themeElements>
-    <a:clrScheme name="LibreOffice">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="000000"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="ffffff"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="18a303"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="0369a3"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="a33e03"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8e03a3"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="c99c00"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="c9211e"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000ee"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="551a8b"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="A7:E15"/>
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.25"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.24"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -517,10 +423,129 @@
         <v>13</v>
       </c>
     </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>0.671</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>-8</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>0.633</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>-14</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>-20</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>0.535</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>-38</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>-17</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>0.671</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>-8</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>0.633</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>-11</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>-4</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPágina &amp;P</oddFooter>

</xml_diff>

<commit_message>
Fixed bug in create_def
</commit_message>
<xml_diff>
--- a/scripts_python/references/ref_MD_backup.xlsx
+++ b/scripts_python/references/ref_MD_backup.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="11">
   <si>
     <t xml:space="preserve">Referencias</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t xml:space="preserve">CaCu5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Li3Bi</t>
   </si>
 </sst>
 </file>
@@ -130,313 +133,419 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
+      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.24"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="1" width="11.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B2" s="2" t="n">
         <v>0.423</v>
       </c>
-      <c r="C2" s="1" t="n">
+      <c r="C2" s="2" t="n">
         <v>46</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="D2" s="2" t="n">
         <v>-94</v>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="E2" s="2" t="n">
         <v>-50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="n">
+      <c r="B3" s="2" t="n">
         <v>0.47</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="C3" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="D3" s="2" t="n">
         <v>-48</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="E3" s="2" t="n">
         <v>-36</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="n">
+      <c r="B4" s="2" t="n">
         <v>0.511</v>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="C4" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="D4" s="2" t="n">
         <v>-29</v>
       </c>
-      <c r="E4" s="1" t="n">
+      <c r="E4" s="2" t="n">
         <v>-16</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1" t="n">
+      <c r="B5" s="2" t="n">
         <v>0.73</v>
       </c>
-      <c r="C5" s="1" t="n">
+      <c r="C5" s="2" t="n">
         <v>-16</v>
       </c>
-      <c r="D5" s="1" t="n">
+      <c r="D5" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="E5" s="1" t="n">
+      <c r="E5" s="2" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="1" t="n">
+      <c r="B6" s="2" t="n">
         <v>0.76</v>
       </c>
-      <c r="C6" s="1" t="n">
+      <c r="C6" s="2" t="n">
         <v>-14</v>
       </c>
-      <c r="D6" s="1" t="n">
+      <c r="D6" s="2" t="n">
         <v>18</v>
       </c>
-      <c r="E6" s="1" t="n">
+      <c r="E6" s="2" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="0" t="n">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="n">
         <v>0.92</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <v>-4</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="0" t="n">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="n">
         <v>0.852</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="1" t="n">
         <v>-10</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="1" t="n">
         <v>-1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="0" t="n">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="n">
         <v>0.815</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="1" t="n">
         <v>-8</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="1" t="n">
         <v>-3</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="0" t="n">
+      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1" t="n">
         <v>0.782</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="1" t="n">
         <v>-1</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="1" t="n">
         <v>-4</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="0" t="n">
+      <c r="A11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="1" t="n">
         <v>0.69</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="1" t="n">
         <v>-4</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="1" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="0" t="n">
+      <c r="A12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="1" t="n">
         <v>0.758</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12" s="1" t="n">
         <v>-19</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D12" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12" s="1" t="n">
         <v>-7</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="0" t="n">
+      <c r="A13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="1" t="n">
         <v>0.692</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="C13" s="1" t="n">
         <v>-24</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="D13" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13" s="1" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="0" t="n">
+      <c r="A14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="1" t="n">
         <v>0.797</v>
       </c>
-      <c r="C14" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="D14" s="0" t="n">
+      <c r="C14" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="D14" s="1" t="n">
         <v>-19</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14" s="1" t="n">
         <v>-9</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="0" t="n">
+      <c r="A15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="1" t="n">
         <v>0.673</v>
       </c>
-      <c r="C15" s="0" t="n">
+      <c r="C15" s="1" t="n">
         <v>-16</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15" s="1" t="n">
         <v>13</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="0" t="n">
+      <c r="B16" s="1" t="n">
         <v>0.671</v>
       </c>
-      <c r="C16" s="0" t="n">
+      <c r="C16" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D16" s="1" t="n">
         <v>-8</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="E16" s="1" t="n">
         <v>2</v>
       </c>
     </row>
@@ -444,16 +553,16 @@
       <c r="A17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="0" t="n">
+      <c r="B17" s="1" t="n">
         <v>0.633</v>
       </c>
-      <c r="C17" s="0" t="n">
+      <c r="C17" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="D17" s="1" t="n">
         <v>-14</v>
       </c>
-      <c r="E17" s="0" t="n">
+      <c r="E17" s="1" t="n">
         <v>-1</v>
       </c>
     </row>
@@ -461,16 +570,16 @@
       <c r="A18" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="0" t="n">
+      <c r="B18" s="1" t="n">
         <v>0.58</v>
       </c>
-      <c r="C18" s="0" t="n">
+      <c r="C18" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="D18" s="0" t="n">
+      <c r="D18" s="1" t="n">
         <v>-20</v>
       </c>
-      <c r="E18" s="0" t="n">
+      <c r="E18" s="1" t="n">
         <v>-3</v>
       </c>
     </row>
@@ -478,16 +587,16 @@
       <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="0" t="n">
+      <c r="B19" s="1" t="n">
         <v>0.535</v>
       </c>
-      <c r="C19" s="0" t="n">
+      <c r="C19" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="D19" s="0" t="n">
+      <c r="D19" s="1" t="n">
         <v>-38</v>
       </c>
-      <c r="E19" s="0" t="n">
+      <c r="E19" s="1" t="n">
         <v>-17</v>
       </c>
     </row>
@@ -495,16 +604,16 @@
       <c r="A20" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="0" t="n">
+      <c r="B20" s="1" t="n">
         <v>0.671</v>
       </c>
-      <c r="C20" s="0" t="n">
+      <c r="C20" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="D20" s="0" t="n">
+      <c r="D20" s="1" t="n">
         <v>-8</v>
       </c>
-      <c r="E20" s="0" t="n">
+      <c r="E20" s="1" t="n">
         <v>-1</v>
       </c>
     </row>
@@ -512,16 +621,16 @@
       <c r="A21" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="0" t="n">
+      <c r="B21" s="1" t="n">
         <v>0.633</v>
       </c>
-      <c r="C21" s="0" t="n">
+      <c r="C21" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="D21" s="0" t="n">
+      <c r="D21" s="1" t="n">
         <v>-11</v>
       </c>
-      <c r="E21" s="0" t="n">
+      <c r="E21" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -529,23 +638,74 @@
       <c r="A22" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="0" t="n">
+      <c r="B22" s="1" t="n">
         <v>0.58</v>
       </c>
-      <c r="C22" s="0" t="n">
+      <c r="C22" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="D22" s="0" t="n">
+      <c r="D22" s="1" t="n">
         <v>-4</v>
       </c>
-      <c r="E22" s="0" t="n">
+      <c r="E22" s="1" t="n">
         <v>6</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="1" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="C23" s="1" t="n">
+        <v>-6</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="E23" s="1" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="1" t="n">
+        <v>0.535</v>
+      </c>
+      <c r="C24" s="1" t="n">
+        <v>-18</v>
+      </c>
+      <c r="D24" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="E24" s="1" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="1" t="n">
+        <v>0.566</v>
+      </c>
+      <c r="C25" s="1" t="n">
+        <v>-54</v>
+      </c>
+      <c r="D25" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="E25" s="1" t="n">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPágina &amp;P</oddFooter>

</xml_diff>

<commit_message>
Added full compatibility with NaZn13.
</commit_message>
<xml_diff>
--- a/scripts_python/references/ref_MD_backup.xlsx
+++ b/scripts_python/references/ref_MD_backup.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="13">
   <si>
     <t xml:space="preserve">Referencias</t>
   </si>
@@ -53,6 +53,12 @@
   </si>
   <si>
     <t xml:space="preserve">Li3Bi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cu3Au</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NaZn13</t>
   </si>
 </sst>
 </file>
@@ -264,10 +270,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
+      <selection pane="topLeft" activeCell="H31" activeCellId="0" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -702,6 +708,159 @@
         <v>16</v>
       </c>
     </row>
+    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" s="1" t="n">
+        <v>0.633</v>
+      </c>
+      <c r="C26" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="D26" s="1" t="n">
+        <v>-3</v>
+      </c>
+      <c r="E26" s="1" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="1" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="C27" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="D27" s="1" t="n">
+        <v>-6</v>
+      </c>
+      <c r="E27" s="1" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" s="1" t="n">
+        <v>0.535</v>
+      </c>
+      <c r="C28" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="D28" s="1" t="n">
+        <v>-2</v>
+      </c>
+      <c r="E28" s="1" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" s="1" t="n">
+        <v>0.486</v>
+      </c>
+      <c r="C29" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="D29" s="1" t="n">
+        <v>-15</v>
+      </c>
+      <c r="E29" s="1" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" s="1" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="C30" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="D30" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="E30" s="1" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" s="1" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="C31" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="D31" s="1" t="n">
+        <v>-5</v>
+      </c>
+      <c r="E31" s="1" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" s="1" t="n">
+        <v>0.658</v>
+      </c>
+      <c r="C32" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="D32" s="1" t="n">
+        <v>-10</v>
+      </c>
+      <c r="E32" s="1" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33" s="1" t="n">
+        <v>0.633</v>
+      </c>
+      <c r="C33" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="D33" s="1" t="n">
+        <v>-8</v>
+      </c>
+      <c r="E33" s="1" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="1" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="C34" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="D34" s="1" t="n">
+        <v>-10</v>
+      </c>
+      <c r="E34" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Added CaB6 and Fe4C references.
</commit_message>
<xml_diff>
--- a/scripts_python/references/ref_MD_backup.xlsx
+++ b/scripts_python/references/ref_MD_backup.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="15">
   <si>
     <t xml:space="preserve">Referencias</t>
   </si>
@@ -59,6 +59,12 @@
   </si>
   <si>
     <t xml:space="preserve">NaZn13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CaB6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fe4C</t>
   </si>
 </sst>
 </file>
@@ -270,10 +276,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H31" activeCellId="0" sqref="H31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A40" activeCellId="0" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -861,6 +867,108 @@
         <v>0</v>
       </c>
     </row>
+    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="1" t="n">
+        <v>0.535</v>
+      </c>
+      <c r="C35" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="D35" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="E35" s="1" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36" s="1" t="n">
+        <v>0.486</v>
+      </c>
+      <c r="C36" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="D36" s="1" t="n">
+        <v>-3</v>
+      </c>
+      <c r="E36" s="1" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B37" s="1" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="C37" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="D37" s="1" t="n">
+        <v>-21</v>
+      </c>
+      <c r="E37" s="1" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" s="1" t="n">
+        <v>0.535</v>
+      </c>
+      <c r="C38" s="1" t="n">
+        <v>112</v>
+      </c>
+      <c r="D38" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E38" s="1" t="n">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" s="1" t="n">
+        <v>0.486</v>
+      </c>
+      <c r="C39" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="D39" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="E39" s="1" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B40" s="1" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="C40" s="1" t="n">
+        <v>-32</v>
+      </c>
+      <c r="D40" s="1" t="n">
+        <v>108</v>
+      </c>
+      <c r="E40" s="1" t="n">
+        <v>77</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>